<commit_message>
commitando a massa de dados
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub_tdd/appium/dadosParaTeste/DadosParaTeste.xlsx
+++ b/src/main/java/br/com/rsinet/hub_tdd/appium/dadosParaTeste/DadosParaTeste.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Workspace\AppiumTDD\src\main\java\br\com\rsinet\hub_tdd\appium\dadosParaTeste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0093B8FC-3D73-4412-A7DC-EECB3DA7B6B7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58437C0C-D568-4A5A-8712-2F93D3047896}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15420" yWindow="1155" windowWidth="15375" windowHeight="7875" xr2:uid="{AACC88D3-5814-4D61-8B68-BC0AA92C6385}"/>
+    <workbookView xWindow="-20520" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="2" xr2:uid="{AACC88D3-5814-4D61-8B68-BC0AA92C6385}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
     <sheet name="Pesquisar pela barra" sheetId="2" r:id="rId2"/>
+    <sheet name="Pesquisa pela tela" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="106">
   <si>
     <t>Username</t>
   </si>
@@ -91,9 +92,6 @@
     <t>Cadastro</t>
   </si>
   <si>
-    <t>Buscar Produto</t>
-  </si>
-  <si>
     <t>mouse</t>
   </si>
   <si>
@@ -334,7 +332,25 @@
     <t>a</t>
   </si>
   <si>
-    <t>qwpwfi</t>
+    <t>qpwifon</t>
+  </si>
+  <si>
+    <t>Pesquisar pela barra</t>
+  </si>
+  <si>
+    <t>roupa</t>
+  </si>
+  <si>
+    <t>Pesquisar pela tela</t>
+  </si>
+  <si>
+    <t>headphone</t>
+  </si>
+  <si>
+    <t>BEATS STUDIO 2 OVER-EAR MATTE</t>
+  </si>
+  <si>
+    <t>BOSE SOUNDLINK AROUND-EAR</t>
   </si>
 </sst>
 </file>
@@ -747,7 +763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C2567E2-D904-4AF5-AA09-5D36B24D5ECF}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -774,7 +790,7 @@
         <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -815,25 +831,25 @@
         <v>18</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>14</v>
@@ -842,13 +858,13 @@
         <v>15</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -856,19 +872,19 @@
         <v>18</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>12</v>
@@ -883,13 +899,13 @@
         <v>15</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -897,40 +913,40 @@
         <v>18</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -938,40 +954,40 @@
         <v>18</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -979,40 +995,40 @@
         <v>18</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1020,40 +1036,40 @@
         <v>18</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1061,40 +1077,40 @@
         <v>18</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1102,19 +1118,19 @@
         <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>12</v>
@@ -1123,16 +1139,16 @@
         <v>13</v>
       </c>
       <c r="I9" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="J9" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="J9" s="5" t="s">
-        <v>79</v>
-      </c>
       <c r="K9" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M9" s="5" t="s">
         <v>16</v>
@@ -1176,12 +1192,12 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.85546875" bestFit="1" customWidth="1"/>
@@ -1192,45 +1208,107 @@
         <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="N1" s="6"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N2" s="6"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>19</v>
+        <v>100</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="N3" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D8C683-B5E6-4D46-94DE-AF4F982BB4CB}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="D3" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="N3" s="6"/>
+        <v>105</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>